<commit_message>
new calc with another specs
</commit_message>
<xml_diff>
--- a/profiles_u.xlsx
+++ b/profiles_u.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuva\Документы\GitHub\My_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD978D9-DA6B-4B2B-9CB6-C61C749A695A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CC52B5-17B8-4BB7-A9AE-31F887C56143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2717,8 +2717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408FD670-9089-40E6-AE6C-6BD978CBF367}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18:J31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2754,19 +2754,19 @@
         <v>1480</v>
       </c>
       <c r="C2">
-        <v>64.470993381750702</v>
+        <v>45.843044735101898</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>26.5811482268142</v>
+        <v>72.702517806361399</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>39.993013320879797</v>
+        <v>40.030768539705598</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2777,16 +2777,16 @@
         <v>1480</v>
       </c>
       <c r="C3">
-        <v>81.770450640149406</v>
+        <v>51.184873684844099</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.60249050796316295</v>
+        <v>68.030313027219606</v>
       </c>
       <c r="F3">
-        <v>66.574172930233203</v>
+        <v>112.733548501862</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2800,16 +2800,16 @@
         <v>1480</v>
       </c>
       <c r="C4">
-        <v>82.094276447300103</v>
+        <v>58.989560837636503</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.42958755490372802</v>
+        <v>63.983343633597997</v>
       </c>
       <c r="F4">
-        <v>40.5955152113822</v>
+        <v>108.06134372272101</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2823,16 +2823,16 @@
         <v>1480</v>
       </c>
       <c r="C5">
-        <v>82.007258711811602</v>
+        <v>66.962464918358805</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.423332256748294</v>
+        <v>61.410091724147499</v>
       </c>
       <c r="F5">
-        <v>40.4226122583228</v>
+        <v>104.014374329099</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2846,16 +2846,16 @@
         <v>1480</v>
       </c>
       <c r="C6">
-        <v>82.002600627358305</v>
+        <v>73.1831060549368</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>7.7435617703909099</v>
+        <v>59.318087283870497</v>
       </c>
       <c r="F6">
-        <v>40.416356960167398</v>
+        <v>101.44112241964901</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2869,16 +2869,16 @@
         <v>1480</v>
       </c>
       <c r="C7">
-        <v>85.264462469887903</v>
+        <v>77.905954779800695</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>4.30801871094768</v>
+        <v>57.175327782790397</v>
       </c>
       <c r="F7">
-        <v>47.73658647381</v>
+        <v>99.349117979371499</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2892,16 +2892,16 @@
         <v>1480</v>
       </c>
       <c r="C8">
-        <v>84.307166563105895</v>
+        <v>82.584114548625493</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8">
-        <v>60.460063701243897</v>
+        <v>102.751525039432</v>
       </c>
       <c r="F8">
-        <v>44.301043414366802</v>
+        <v>97.206358478291506</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2915,16 +2915,16 @@
         <v>1480</v>
       </c>
       <c r="C9">
-        <v>84.301898942681902</v>
+        <v>83.214022553712397</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>60.475060782938897</v>
+        <v>102.836422335138</v>
       </c>
       <c r="F9">
-        <v>0.45308840466292599</v>
+        <v>42.782555734933503</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -2938,16 +2938,16 @@
         <v>1480</v>
       </c>
       <c r="C10">
-        <v>84.286894745684506</v>
+        <v>84.266577128667805</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>60.4986949021878</v>
+        <v>102.91888984825501</v>
       </c>
       <c r="F10">
-        <v>0.46808548635795699</v>
+        <v>42.867453030639503</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -2961,16 +2961,16 @@
         <v>1480</v>
       </c>
       <c r="C11">
-        <v>83.5358448868799</v>
+        <v>85.928579906131503</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>62.5906098828642</v>
+        <v>103.14747230052301</v>
       </c>
       <c r="F11">
-        <v>0.49171960560686501</v>
+        <v>42.949920543755603</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2984,16 +2984,16 @@
         <v>1480</v>
       </c>
       <c r="C12">
-        <v>82.799530113498605</v>
+        <v>88.422082572867197</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>64.779163394916395</v>
+        <v>103.57286700243201</v>
       </c>
       <c r="F12">
-        <v>2.5836345862832699</v>
+        <v>43.1785029960241</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3007,16 +3007,16 @@
         <v>1480</v>
       </c>
       <c r="C13">
-        <v>82.616629586439899</v>
+        <v>91.893430952109597</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>65.136068103680799</v>
+        <v>104.365184854777</v>
       </c>
       <c r="F13">
-        <v>4.7721880983354499</v>
+        <v>43.603897697933199</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -3030,16 +3030,16 @@
         <v>1480</v>
       </c>
       <c r="C14">
-        <v>81.767953141825004</v>
+        <v>96.487399373042606</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>69.158967020116293</v>
+        <v>105.268123611501</v>
       </c>
       <c r="F14">
-        <v>5.1290928070998296</v>
+        <v>44.396215550277603</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3053,7 +3053,7 @@
         <v>1480</v>
       </c>
       <c r="C15">
-        <v>84.463369514128502</v>
+        <v>102.968089319798</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -3062,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>9.15199172353541</v>
+        <v>45.2991543070017</v>
       </c>
       <c r="G15">
-        <v>60.006975296580897</v>
+        <v>59.968969304498998</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3081,19 +3081,19 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.55597000267654295</v>
+        <v>0.92341645680734197</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18">
-        <v>0.34714304728652801</v>
+      <c r="E18" s="1">
+        <v>7.6372996643049806E-2</v>
       </c>
       <c r="F18" s="1">
-        <v>5.2920571368660498E-2</v>
+        <v>1.4722195819304599E-4</v>
       </c>
       <c r="G18" s="1">
-        <v>4.3966378668269301E-2</v>
+        <v>6.3324591415662204E-5</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -3113,19 +3113,19 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0.32207590670362002</v>
+        <v>0.77642845886959799</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.441101740569458</v>
-      </c>
-      <c r="F19">
-        <v>0.11879752999927</v>
-      </c>
-      <c r="G19">
-        <v>0.118024822727652</v>
+        <v>0.22193146909873099</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.0641259123113E-3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5.7594611935899505E-4</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -3145,19 +3145,19 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.31881823579703</v>
+        <v>0.59319158667921801</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.440634343009082</v>
-      </c>
-      <c r="F20">
-        <v>0.120316130413929</v>
-      </c>
-      <c r="G20">
-        <v>0.120231290779959</v>
+        <v>0.39997784288323501</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4.1649786106610302E-3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2.6655918268866001E-3</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -3177,19 +3177,19 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.319701137873247</v>
+        <v>0.43870100361966902</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.44072652299547699</v>
-      </c>
-      <c r="F21">
-        <v>0.119912996238831</v>
-      </c>
-      <c r="G21">
-        <v>0.11965934289244499</v>
+        <v>0.54040170042507996</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.20856383446165E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>8.8116576106348002E-3</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -3209,19 +3209,19 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.31974547442012902</v>
+        <v>0.34122979930113501</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0.440741745241788</v>
-      </c>
-      <c r="F22">
-        <v>0.119890071712994</v>
-      </c>
-      <c r="G22">
-        <v>0.119622708625089</v>
+        <v>0.60632381605219099</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2.8968287552830901E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2.3478097093843599E-2</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -3241,19 +3241,19 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>0.28773179067702798</v>
+        <v>0.28697362316793301</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0.43614493903313001</v>
-      </c>
-      <c r="F23">
-        <v>0.13481704954832799</v>
-      </c>
-      <c r="G23">
-        <v>0.141306220741514</v>
+        <v>0.59801094565313495</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6.0768490900736702E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5.4246940278195897E-2</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3273,19 +3273,19 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>0.29780308833611402</v>
+        <v>0.25314714171111902</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0.43463216353640199</v>
+        <v>0.52352089442333205</v>
       </c>
       <c r="F24">
-        <v>0.13084879512504</v>
+        <v>0.11245012503275301</v>
       </c>
       <c r="G24">
-        <v>0.13671595300244299</v>
+        <v>0.110881838832796</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -3305,19 +3305,19 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0.29786238072643401</v>
+        <v>0.24488126999719401</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0.43461142751937198</v>
+        <v>0.53094323079121197</v>
       </c>
       <c r="F25">
-        <v>0.13083116030846301</v>
+        <v>0.112863047513557</v>
       </c>
       <c r="G25">
-        <v>0.136695031445731</v>
+        <v>0.111312451698037</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -3337,19 +3337,19 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0.29803823351891801</v>
+        <v>0.231270673323762</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0.43452661424976702</v>
+        <v>0.54310246620496405</v>
       </c>
       <c r="F26">
-        <v>0.13078803646213</v>
+        <v>0.113571047277228</v>
       </c>
       <c r="G26">
-        <v>0.13664711576918401</v>
+        <v>0.11205581319404501</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -3369,19 +3369,19 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>0.30656700496483902</v>
+        <v>0.21024267634221899</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0.43139922047121598</v>
+        <v>0.56193568092351198</v>
       </c>
       <c r="F27">
-        <v>0.12830781273432099</v>
+        <v>0.11463935994112399</v>
       </c>
       <c r="G27">
-        <v>0.13372596182962401</v>
+        <v>0.113182282793145</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -3401,19 +3401,19 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>0.31501200518382999</v>
+        <v>0.17988342877967001</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.42826527448554702</v>
+        <v>0.58874471688637098</v>
       </c>
       <c r="F28">
-        <v>0.12586697051665999</v>
+        <v>0.116380707820948</v>
       </c>
       <c r="G28">
-        <v>0.130855749813964</v>
+        <v>0.114991146513011</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -3433,19 +3433,19 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0.317177328813319</v>
+        <v>0.14039630587152899</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0.42728344834040399</v>
+        <v>0.62107695299247201</v>
       </c>
       <c r="F29">
-        <v>0.125308759784971</v>
+        <v>0.119960893647338</v>
       </c>
       <c r="G29">
-        <v>0.13023046306130601</v>
+        <v>0.118565847488661</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -3464,20 +3464,20 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
-        <v>0.32670792295920398</v>
+      <c r="C30" s="1">
+        <v>9.5169982630262898E-2</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.42489456277968102</v>
+        <v>0.6449405675598</v>
       </c>
       <c r="F30">
-        <v>0.1221033656603</v>
+        <v>0.13069459332730601</v>
       </c>
       <c r="G30">
-        <v>0.126294148600815</v>
+        <v>0.12919485648263199</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -3496,20 +3496,20 @@
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31">
-        <v>0.29605017529863598</v>
+      <c r="C31" s="1">
+        <v>5.0604060890918602E-2</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0.43522775514652601</v>
+        <v>0.61603066894303704</v>
       </c>
       <c r="F31">
-        <v>0.13137717157200099</v>
+        <v>0.166654633275337</v>
       </c>
       <c r="G31">
-        <v>0.137344897982837</v>
+        <v>0.166710636890707</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -3534,19 +3534,19 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>0.76619579584992503</v>
+        <v>0.97719579056403705</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34">
-        <v>0.20506453708146599</v>
+      <c r="E34" s="1">
+        <v>2.27811992568735E-2</v>
       </c>
       <c r="F34" s="1">
-        <v>1.7153367175238202E-2</v>
+        <v>1.7266034568324799E-5</v>
       </c>
       <c r="G34" s="1">
-        <v>1.1586299893370899E-2</v>
+        <v>5.7441445206971796E-6</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -3566,19 +3566,19 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>0.55597003861996097</v>
+        <v>0.92341658186828601</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="E35">
-        <v>0.34714302299461203</v>
-      </c>
-      <c r="F35">
-        <v>5.2920565253352002E-2</v>
+      <c r="E35" s="1">
+        <v>7.6372872018211302E-2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1.47221655987545E-4</v>
       </c>
       <c r="G35" s="1">
-        <v>4.3966373132075597E-2</v>
+        <v>6.3324457515434194E-5</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3598,19 +3598,19 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0.552498767515338</v>
+        <v>0.83087989314917099</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0.34853747727059398</v>
+        <v>0.168009599098527</v>
       </c>
       <c r="F36" s="1">
-        <v>5.3898261513499197E-2</v>
-      </c>
-      <c r="G36">
-        <v>4.5065493700568997E-2</v>
+        <v>7.2446102257038797E-4</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3.86046729731033E-4</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3630,19 +3630,19 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>0.55344975351202796</v>
+        <v>0.72028225175648297</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0.34813657733509001</v>
+        <v>0.27543496440119802</v>
       </c>
       <c r="F37" s="1">
-        <v>5.3636801337050503E-2</v>
+        <v>2.6187021946550999E-3</v>
       </c>
       <c r="G37" s="1">
-        <v>4.4776867815831699E-2</v>
+        <v>1.6640816476638199E-3</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -3662,19 +3662,19 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>0.55349531553609199</v>
+        <v>0.62998115530640797</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0.34812322684083702</v>
+        <v>0.35728502258265998</v>
       </c>
       <c r="F38" s="1">
-        <v>5.3622258740228197E-2</v>
+        <v>7.3744607128051398E-3</v>
       </c>
       <c r="G38" s="1">
-        <v>4.4759198882843597E-2</v>
+        <v>5.3593613981271796E-3</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -3694,19 +3694,19 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>0.51765103250184796</v>
+        <v>0.57581211396793597</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0.36232607011175899</v>
+        <v>0.39278904091026701</v>
       </c>
       <c r="F39" s="1">
-        <v>6.3783980209413393E-2</v>
+        <v>1.73553309505966E-2</v>
       </c>
       <c r="G39" s="1">
-        <v>5.6238917176979299E-2</v>
+        <v>1.40435141711997E-2</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3726,19 +3726,19 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>0.52988545129085296</v>
+        <v>0.54907043562701296</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>0.355797926905357</v>
+        <v>0.38319250038831598</v>
       </c>
       <c r="F40" s="1">
-        <v>6.0884518175446101E-2</v>
+        <v>3.5803746311010798E-2</v>
       </c>
       <c r="G40" s="1">
-        <v>5.3432103628343802E-2</v>
+        <v>3.1933317673660498E-2</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -3758,19 +3758,19 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0.52995868590699402</v>
+        <v>0.53705490710502701</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0.35575208038331002</v>
+        <v>0.39384851433201501</v>
       </c>
       <c r="F41" s="1">
-        <v>6.0870680316226097E-2</v>
-      </c>
-      <c r="G41">
-        <v>5.341855339347E-2</v>
+        <v>3.6470828445036602E-2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3.2625750117921702E-2</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3790,19 +3790,19 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>0.53018098386086299</v>
+        <v>0.51666331361734197</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0.35560031144100501</v>
+        <v>0.41191106055524901</v>
       </c>
       <c r="F42">
-        <v>6.0834364087119001E-2</v>
+        <v>3.7611878448700002E-2</v>
       </c>
       <c r="G42" s="1">
-        <v>5.3384340611013402E-2</v>
+        <v>3.3813747378708903E-2</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3822,19 +3822,19 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0.54065081018318495</v>
+        <v>0.48352703138373498</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0.34896292309028898</v>
+        <v>0.44127622075297801</v>
       </c>
       <c r="F43" s="1">
-        <v>5.8892965406950097E-2</v>
+        <v>3.9452913902563599E-2</v>
       </c>
       <c r="G43" s="1">
-        <v>5.1493301319575503E-2</v>
+        <v>3.5743833960722997E-2</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3854,19 +3854,19 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>0.55082876757191601</v>
+        <v>0.43195863603385598</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0.342478447037117</v>
+        <v>0.48680522361310402</v>
       </c>
       <c r="F44" s="1">
-        <v>5.7019504036626902E-2</v>
+        <v>4.2397338715149599E-2</v>
       </c>
       <c r="G44" s="1">
-        <v>4.9673281354339897E-2</v>
+        <v>3.8838801637889497E-2</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3886,19 +3886,19 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>0.55344394333304803</v>
+        <v>0.35768291125559099</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0.340716880244335</v>
+        <v>0.55121801611604604</v>
       </c>
       <c r="F45" s="1">
-        <v>5.65799910863376E-2</v>
+        <v>4.7238368453110698E-2</v>
       </c>
       <c r="G45" s="1">
-        <v>4.9259185336279099E-2</v>
+        <v>4.3860704175251897E-2</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3918,19 +3918,19 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>0.56435097661468303</v>
+        <v>0.26168476067070401</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.33434034120779299</v>
+        <v>0.62789330996144899</v>
       </c>
       <c r="F46" s="1">
-        <v>5.4312377015346698E-2</v>
+        <v>5.6888503269996497E-2</v>
       </c>
       <c r="G46" s="1">
-        <v>4.6996305162177399E-2</v>
+        <v>5.3533426097851299E-2</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3950,19 +3950,19 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>0.52772194942357697</v>
+        <v>0.15416826711700801</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>0.35714279487789602</v>
+        <v>0.68321273509288905</v>
       </c>
       <c r="F47" s="1">
-        <v>6.1297689796582601E-2</v>
+        <v>8.3089145392955505E-2</v>
       </c>
       <c r="G47" s="1">
-        <v>5.3837565901944599E-2</v>
+        <v>7.9529852397147396E-2</v>
       </c>
       <c r="H47">
         <v>0</v>

</xml_diff>